<commit_message>
Added support for Floating Holidays
</commit_message>
<xml_diff>
--- a/Dynamic Event Calendar Template.xlsx
+++ b/Dynamic Event Calendar Template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145FCCCC-105F-4E1D-8F50-C0599C73E1B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC256F39-970A-428E-9B0A-FDF5BE33F7D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="788" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="788" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="26" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
   <si>
     <t>NOTES</t>
   </si>
@@ -197,22 +197,31 @@
     <t>Mashirao Ojiro</t>
   </si>
   <si>
-    <t>Column1</t>
+    <t>Christmas</t>
   </si>
   <si>
-    <t>Sum</t>
+    <t>Martin Luther King Jr. Day</t>
   </si>
   <si>
-    <t>Average</t>
+    <t>Daylight Savings Starts</t>
   </si>
   <si>
-    <t>Running Total</t>
+    <t>Mother's Day</t>
   </si>
   <si>
-    <t>Count</t>
+    <t>Memorial Day</t>
   </si>
   <si>
-    <t>Christmas</t>
+    <t>Father's Day</t>
+  </si>
+  <si>
+    <t>Labor Day</t>
+  </si>
+  <si>
+    <t>Daylight Savings Ends</t>
+  </si>
+  <si>
+    <t>Thanksgiving</t>
   </si>
 </sst>
 </file>
@@ -418,7 +427,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -507,6 +516,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -519,7 +537,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -625,7 +643,9 @@
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -633,6 +653,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -646,59 +675,6 @@
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="30">
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Sylfaen"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <color theme="0" tint="-0.24994659260841701"/>
@@ -819,6 +795,59 @@
         <color theme="0" tint="-0.24994659260841701"/>
       </font>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Sylfaen"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -932,7 +961,7 @@
                   <a14:compatExt spid="_x0000_s1038"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000E040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -963,15 +992,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{032961F6-0716-462B-8D1D-12ED5EF2231F}" name="plan" displayName="plan" ref="A2:D37" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A2:D37" xr:uid="{032961F6-0716-462B-8D1D-12ED5EF2231F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{032961F6-0716-462B-8D1D-12ED5EF2231F}" name="plan" displayName="plan" ref="A2:D46" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+  <autoFilter ref="A2:D46" xr:uid="{032961F6-0716-462B-8D1D-12ED5EF2231F}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{71ABF3BA-24C3-463A-96A5-E0B1588A0D0D}" name="Date" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{0499C450-05BA-4BC0-8200-BA2057209A7A}" name="Event" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{71ABF3BA-24C3-463A-96A5-E0B1588A0D0D}" name="Date" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{0499C450-05BA-4BC0-8200-BA2057209A7A}" name="Event" dataDxfId="26">
       <calculatedColumnFormula>_xlfn.TEXTJOIN("",FALSE,C3,"'s ",CalendarYear - D3,IF(RIGHT(CalendarYear - D3,1)="1","st",IF(RIGHT(CalendarYear - D3,1)="2","nd",IF(RIGHT(CalendarYear - D3,1)="3","rd","th")))," Birthday")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B767956B-8230-44B9-BF7F-73015F4D6D91}" name="Name" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{DEDC8ED6-E783-428A-B298-50ADDDE75BB5}" name="Year" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{B767956B-8230-44B9-BF7F-73015F4D6D91}" name="Name" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{DEDC8ED6-E783-428A-B298-50ADDDE75BB5}" name="Year" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1206,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3176040A-2F43-494E-AE28-219FF4000FEE}">
   <dimension ref="A1:D247"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1284,7 +1313,7 @@
         <f>plan[[#This Row],[Name]]</f>
         <v>Saint Patrick's Day</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -1300,7 +1329,7 @@
         <f>plan[[#This Row],[Name]]</f>
         <v>Fourth of July</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="20" t="s">
@@ -1332,8 +1361,8 @@
         <f>plan[[#This Row],[Name]]</f>
         <v>Christmas</v>
       </c>
-      <c r="C8" s="39" t="s">
-        <v>44</v>
+      <c r="C8" t="s">
+        <v>39</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>10</v>
@@ -1391,366 +1420,473 @@
       <c r="C12" s="28"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C13" s="25"/>
+      <c r="A13" s="21">
+        <f>DATE(CalendarYear,1,1+7*3)-WEEKDAY(DATE(CalendarYear,1,8-2))</f>
+        <v>44578</v>
+      </c>
+      <c r="B13" s="18" t="str">
+        <f>plan[[#This Row],[Name]]</f>
+        <v>Martin Luther King Jr. Day</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C14" s="28"/>
+      <c r="A14" s="21">
+        <f>DATE(CalendarYear,3,1+7*2)-WEEKDAY(DATE(CalendarYear,3,8-1))</f>
+        <v>44633</v>
+      </c>
+      <c r="B14" s="18" t="str">
+        <f>plan[[#This Row],[Name]]</f>
+        <v>Daylight Savings Starts</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="21">
+        <f>DATE(CalendarYear,5,1+7*2)-WEEKDAY(DATE(CalendarYear,5,8-1))</f>
+        <v>44689</v>
+      </c>
+      <c r="B15" s="18" t="str">
+        <f>plan[[#This Row],[Name]]</f>
+        <v>Mother's Day</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="21">
+        <f>DATE(CalendarYear,5,1+7*5)-WEEKDAY(DATE(CalendarYear,5,8-2))</f>
+        <v>44711</v>
+      </c>
+      <c r="B16" s="18" t="str">
+        <f>plan[[#This Row],[Name]]</f>
+        <v>Memorial Day</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="21">
+        <f>DATE(CalendarYear,6,1+7*3)-WEEKDAY(DATE(CalendarYear,6,8-1))</f>
+        <v>44731</v>
+      </c>
+      <c r="B17" s="18" t="str">
+        <f>plan[[#This Row],[Name]]</f>
+        <v>Father's Day</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="21">
+        <f>DATE(CalendarYear,9,1+7*1)-WEEKDAY(DATE(CalendarYear,9,8-2))</f>
+        <v>44809</v>
+      </c>
+      <c r="B18" s="18" t="str">
+        <f>plan[[#This Row],[Name]]</f>
+        <v>Labor Day</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="21">
+        <f>DATE(CalendarYear,11,1+7*1)-WEEKDAY(DATE(CalendarYear,11,8-1))</f>
+        <v>44871</v>
+      </c>
+      <c r="B19" s="18" t="str">
+        <f>plan[[#This Row],[Name]]</f>
+        <v>Daylight Savings Ends</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="21">
+        <f>DATE(CalendarYear,12,1+7*4)-WEEKDAY(DATE(CalendarYear,12,8-5))</f>
+        <v>44917</v>
+      </c>
+      <c r="B20" s="18" t="str">
+        <f>plan[[#This Row],[Name]]</f>
+        <v>Thanksgiving</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C21" s="25"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="21">
         <f>DATE(CalendarYear,1,11)</f>
         <v>44572</v>
       </c>
-      <c r="B15" s="18" t="str">
-        <f>_xlfn.TEXTJOIN("",FALSE,C15,"'s ",CalendarYear - D15,IF(RIGHT(CalendarYear - D15,1)="1","st",IF(RIGHT(CalendarYear - D15,1)="2","nd",IF(RIGHT(CalendarYear - D15,1)="3","rd","th")))," Birthday")</f>
+      <c r="B22" s="18" t="str">
+        <f t="shared" ref="B22:B41" si="0">_xlfn.TEXTJOIN("",FALSE,C22,"'s ",CalendarYear - D22,IF(RIGHT(CalendarYear - D22,1)="1","st",IF(RIGHT(CalendarYear - D22,1)="2","nd",IF(RIGHT(CalendarYear - D22,1)="3","rd","th")))," Birthday")</f>
         <v>Shoto Todoroki's 17th Birthday</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C22" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D22" s="20">
         <v>2005</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="21">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="21">
         <f>DATE(CalendarYear,2,1)</f>
         <v>44593</v>
       </c>
-      <c r="B16" s="18" t="str">
-        <f>_xlfn.TEXTJOIN("",FALSE,C16,"'s ",CalendarYear - D16,IF(RIGHT(CalendarYear - D16,1)="1","st",IF(RIGHT(CalendarYear - D16,1)="2","nd",IF(RIGHT(CalendarYear - D16,1)="3","rd","th")))," Birthday")</f>
+      <c r="B23" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>Koji Koda's 17th Birthday</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C23" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D23" s="20">
         <v>2005</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="21">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="21">
         <f>DATE(CalendarYear,2,12)</f>
         <v>44604</v>
       </c>
-      <c r="B17" s="18" t="str">
-        <f>_xlfn.TEXTJOIN("",FALSE,C17,"'s ",CalendarYear - D17,IF(RIGHT(CalendarYear - D17,1)="1","st",IF(RIGHT(CalendarYear - D17,1)="2","nd",IF(RIGHT(CalendarYear - D17,1)="3","rd","th")))," Birthday")</f>
+      <c r="B24" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>Tsuyu Asui's 17th Birthday</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C24" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D24" s="20">
         <v>2005</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="21">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="21">
         <f>DATE(CalendarYear,2,15)</f>
         <v>44607</v>
       </c>
-      <c r="B18" s="18" t="str">
-        <f>_xlfn.TEXTJOIN("",FALSE,C18,"'s ",CalendarYear - D18,IF(RIGHT(CalendarYear - D18,1)="1","st",IF(RIGHT(CalendarYear - D18,1)="2","nd",IF(RIGHT(CalendarYear - D18,1)="3","rd","th")))," Birthday")</f>
+      <c r="B25" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>Mezo Shoji's 17th Birthday</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C25" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="20">
+      <c r="D25" s="20">
         <v>2005</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="21">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="21">
         <f>DATE(CalendarYear,4,20)</f>
         <v>44671</v>
       </c>
-      <c r="B19" s="18" t="str">
-        <f>_xlfn.TEXTJOIN("",FALSE,C19,"'s ",CalendarYear - D19,IF(RIGHT(CalendarYear - D19,1)="1","st",IF(RIGHT(CalendarYear - D19,1)="2","nd",IF(RIGHT(CalendarYear - D19,1)="3","rd","th")))," Birthday")</f>
+      <c r="B26" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>Katsuki Bakugo's 17th Birthday</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C26" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="20">
+      <c r="D26" s="20">
         <v>2005</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="21">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="21">
         <f>DATE(CalendarYear,5,28)</f>
         <v>44709</v>
       </c>
-      <c r="B20" s="18" t="str">
-        <f>_xlfn.TEXTJOIN("",FALSE,C20,"'s ",CalendarYear - D20,IF(RIGHT(CalendarYear - D20,1)="1","st",IF(RIGHT(CalendarYear - D20,1)="2","nd",IF(RIGHT(CalendarYear - D20,1)="3","rd","th")))," Birthday")</f>
+      <c r="B27" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>Mashirao Ojiro's 17th Birthday</v>
       </c>
-      <c r="C20" s="39" t="s">
+      <c r="C27" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D27" s="43">
         <v>2005</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="21">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="21">
         <f>DATE(CalendarYear,5,30)</f>
         <v>44711</v>
       </c>
-      <c r="B21" s="18" t="str">
-        <f>_xlfn.TEXTJOIN("",FALSE,C21,"'s ",CalendarYear - D21,IF(RIGHT(CalendarYear - D21,1)="1","st",IF(RIGHT(CalendarYear - D21,1)="2","nd",IF(RIGHT(CalendarYear - D21,1)="3","rd","th")))," Birthday")</f>
+      <c r="B28" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>Yuga Aoyama's 17th Birthday</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C28" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D28" s="20">
         <v>2005</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="21">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="21">
         <f>DATE(CalendarYear,6,16)</f>
         <v>44728</v>
       </c>
-      <c r="B22" s="18" t="str">
-        <f>_xlfn.TEXTJOIN("",FALSE,C22,"'s ",CalendarYear - D22,IF(RIGHT(CalendarYear - D22,1)="1","st",IF(RIGHT(CalendarYear - D22,1)="2","nd",IF(RIGHT(CalendarYear - D22,1)="3","rd","th")))," Birthday")</f>
+      <c r="B29" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>Toru Hagakure's 17th Birthday</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C29" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="20">
+      <c r="D29" s="20">
         <v>2005</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="21">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="21">
         <f>DATE(CalendarYear,6,19)</f>
         <v>44731</v>
       </c>
-      <c r="B23" s="18" t="str">
-        <f>_xlfn.TEXTJOIN("",FALSE,C23,"'s ",CalendarYear - D23,IF(RIGHT(CalendarYear - D23,1)="1","st",IF(RIGHT(CalendarYear - D23,1)="2","nd",IF(RIGHT(CalendarYear - D23,1)="3","rd","th")))," Birthday")</f>
+      <c r="B30" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>Rikido Sato's 17th Birthday</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C30" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="20">
+      <c r="D30" s="20">
         <v>2005</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="21">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="21">
         <f>DATE(CalendarYear,6,29)</f>
         <v>44741</v>
       </c>
-      <c r="B24" s="18" t="str">
-        <f>_xlfn.TEXTJOIN("",FALSE,C24,"'s ",CalendarYear - D24,IF(RIGHT(CalendarYear - D24,1)="1","st",IF(RIGHT(CalendarYear - D24,1)="2","nd",IF(RIGHT(CalendarYear - D24,1)="3","rd","th")))," Birthday")</f>
+      <c r="B31" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>Denki Kaminari's 17th Birthday</v>
       </c>
-      <c r="C24" s="39" t="s">
+      <c r="C31" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="20">
+      <c r="D31" s="20">
         <v>2005</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="21">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="21">
         <f>DATE(CalendarYear,7,15)</f>
         <v>44757</v>
       </c>
-      <c r="B25" s="18" t="str">
-        <f>_xlfn.TEXTJOIN("",FALSE,C25,"'s ",CalendarYear - D25,IF(RIGHT(CalendarYear - D25,1)="1","st",IF(RIGHT(CalendarYear - D25,1)="2","nd",IF(RIGHT(CalendarYear - D25,1)="3","rd","th")))," Birthday")</f>
+      <c r="B32" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>Izuku Midoriya's 17th Birthday</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C32" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="20">
+      <c r="D32" s="20">
         <v>2005</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="21">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="21">
         <f>DATE(CalendarYear,7,28)</f>
         <v>44770</v>
       </c>
-      <c r="B26" s="18" t="str">
-        <f>_xlfn.TEXTJOIN("",FALSE,C26,"'s ",CalendarYear - D26,IF(RIGHT(CalendarYear - D26,1)="1","st",IF(RIGHT(CalendarYear - D26,1)="2","nd",IF(RIGHT(CalendarYear - D26,1)="3","rd","th")))," Birthday")</f>
+      <c r="B33" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>Hanta Sero's 17th Birthday</v>
       </c>
-      <c r="C26" s="39" t="s">
+      <c r="C33" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="20">
+      <c r="D33" s="20">
         <v>2005</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="21">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="21">
         <f>DATE(CalendarYear,7,30)</f>
         <v>44772</v>
       </c>
-      <c r="B27" s="18" t="str">
-        <f>_xlfn.TEXTJOIN("",FALSE,C27,"'s ",CalendarYear - D27,IF(RIGHT(CalendarYear - D27,1)="1","st",IF(RIGHT(CalendarYear - D27,1)="2","nd",IF(RIGHT(CalendarYear - D27,1)="3","rd","th")))," Birthday")</f>
+      <c r="B34" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>Mina Ashido's 17th Birthday</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C34" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="20">
+      <c r="D34" s="20">
         <v>2005</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="21">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="21">
         <f>DATE(CalendarYear,8,1)</f>
         <v>44774</v>
       </c>
-      <c r="B28" s="18" t="str">
-        <f>_xlfn.TEXTJOIN("",FALSE,C28,"'s ",CalendarYear - D28,IF(RIGHT(CalendarYear - D28,1)="1","st",IF(RIGHT(CalendarYear - D28,1)="2","nd",IF(RIGHT(CalendarYear - D28,1)="3","rd","th")))," Birthday")</f>
+      <c r="B35" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>Kyoka Jiro's 17th Birthday</v>
       </c>
-      <c r="C28" s="39" t="s">
+      <c r="C35" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="20">
+      <c r="D35" s="20">
         <v>2005</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="21">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="21">
         <f>DATE(CalendarYear,8,22)</f>
         <v>44795</v>
       </c>
-      <c r="B29" s="18" t="str">
-        <f>_xlfn.TEXTJOIN("",FALSE,C29,"'s ",CalendarYear - D29,IF(RIGHT(CalendarYear - D29,1)="1","st",IF(RIGHT(CalendarYear - D29,1)="2","nd",IF(RIGHT(CalendarYear - D29,1)="3","rd","th")))," Birthday")</f>
+      <c r="B36" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>Tenya Ida's 17th Birthday</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="C36" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="20">
+      <c r="D36" s="20">
         <v>2005</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="21">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="21">
         <f>DATE(CalendarYear,9,23)</f>
         <v>44827</v>
       </c>
-      <c r="B30" s="18" t="str">
-        <f>_xlfn.TEXTJOIN("",FALSE,C30,"'s ",CalendarYear - D30,IF(RIGHT(CalendarYear - D30,1)="1","st",IF(RIGHT(CalendarYear - D30,1)="2","nd",IF(RIGHT(CalendarYear - D30,1)="3","rd","th")))," Birthday")</f>
+      <c r="B37" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>Momo Yaoyorozu's 17th Birthday</v>
       </c>
-      <c r="C30" s="39" t="s">
+      <c r="C37" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="20">
+      <c r="D37" s="20">
         <v>2005</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="21">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="21">
         <f>DATE(CalendarYear,10,8)</f>
         <v>44842</v>
       </c>
-      <c r="B31" s="18" t="str">
-        <f>_xlfn.TEXTJOIN("",FALSE,C31,"'s ",CalendarYear - D31,IF(RIGHT(CalendarYear - D31,1)="1","st",IF(RIGHT(CalendarYear - D31,1)="2","nd",IF(RIGHT(CalendarYear - D31,1)="3","rd","th")))," Birthday")</f>
+      <c r="B38" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>Minoru Mineta's 17th Birthday</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C38" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="20">
+      <c r="D38" s="20">
         <v>2005</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="21">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="21">
         <f>DATE(CalendarYear,10,16)</f>
         <v>44850</v>
       </c>
-      <c r="B32" s="18" t="str">
-        <f>_xlfn.TEXTJOIN("",FALSE,C32,"'s ",CalendarYear - D32,IF(RIGHT(CalendarYear - D32,1)="1","st",IF(RIGHT(CalendarYear - D32,1)="2","nd",IF(RIGHT(CalendarYear - D32,1)="3","rd","th")))," Birthday")</f>
+      <c r="B39" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>Eijiro Kirishima's 17th Birthday</v>
       </c>
-      <c r="C32" s="39" t="s">
+      <c r="C39" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="20">
+      <c r="D39" s="20">
         <v>2005</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="21">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="21">
         <f>DATE(CalendarYear,10,30)</f>
         <v>44864</v>
       </c>
-      <c r="B33" s="18" t="str">
-        <f>_xlfn.TEXTJOIN("",FALSE,C33,"'s ",CalendarYear - D33,IF(RIGHT(CalendarYear - D33,1)="1","st",IF(RIGHT(CalendarYear - D33,1)="2","nd",IF(RIGHT(CalendarYear - D33,1)="3","rd","th")))," Birthday")</f>
+      <c r="B40" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>Fumikage Tokoyami's 17th Birthday</v>
       </c>
-      <c r="C33" s="25" t="s">
+      <c r="C40" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="20">
+      <c r="D40" s="20">
         <v>2005</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="21">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="21">
         <f>DATE(CalendarYear,12,27)</f>
         <v>44922</v>
       </c>
-      <c r="B34" s="18" t="str">
-        <f>_xlfn.TEXTJOIN("",FALSE,C34,"'s ",CalendarYear - D34,IF(RIGHT(CalendarYear - D34,1)="1","st",IF(RIGHT(CalendarYear - D34,1)="2","nd",IF(RIGHT(CalendarYear - D34,1)="3","rd","th")))," Birthday")</f>
+      <c r="B41" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>Ochaco Uraraka's 17th Birthday</v>
       </c>
-      <c r="C34" s="39" t="s">
+      <c r="C41" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="20">
+      <c r="D41" s="20">
         <v>2005</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C35" s="25"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C36" s="39"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C37" s="25"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C38"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C39"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C40"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C41"/>
-    </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C42"/>
+      <c r="C42" s="44"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C43"/>
+      <c r="C43" s="39"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C44"/>
+      <c r="C44" s="44"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C45"/>
+      <c r="C45" s="39"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C46"/>
+      <c r="A46" s="40"/>
+      <c r="B46" s="41"/>
+      <c r="C46" s="45"/>
+      <c r="D46" s="42"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C47"/>
@@ -1758,58 +1894,52 @@
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C48"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="40"/>
-      <c r="B49" s="41"/>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C49"/>
-      <c r="D49" s="42"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C50"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C51"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C52"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C53"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C54"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="40"/>
-      <c r="B55" s="41"/>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C55"/>
-      <c r="D55" s="42"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C56"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C57"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C58"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C59"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C60"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C61"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C62"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C63"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C64"/>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.3">
@@ -2336,98 +2466,98 @@
     </row>
     <row r="234" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B234" s="20" t="str">
-        <f t="shared" ref="B234:B247" si="0">_xlfn.TEXTJOIN("",FALSE,C234," ",D234)</f>
+        <f t="shared" ref="B234:B247" si="1">_xlfn.TEXTJOIN("",FALSE,C234," ",D234)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C234"/>
     </row>
     <row r="235" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B235" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C235"/>
     </row>
     <row r="236" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B236" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C236"/>
     </row>
     <row r="237" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B237" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C237"/>
     </row>
     <row r="238" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B238" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C238"/>
     </row>
     <row r="239" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B239" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C239"/>
     </row>
     <row r="240" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B240" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C240"/>
     </row>
     <row r="241" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B241" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C241"/>
     </row>
     <row r="242" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B242" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C242"/>
     </row>
     <row r="243" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B243" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C243" s="20"/>
     </row>
     <row r="244" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B244" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C244" s="20"/>
     </row>
     <row r="245" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B245" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C245" s="20"/>
     </row>
     <row r="246" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B246" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C246" s="20"/>
     </row>
     <row r="247" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B247" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C247" s="20"/>
@@ -2438,6 +2568,9 @@
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B3:B11 B13:B20" calculatedColumn="1"/>
+  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -2597,7 +2730,7 @@
       </c>
       <c r="C6" s="16" t="str" cm="1">
         <f t="array" ref="C6">_xlfn.TEXTJOIN(CHAR(10),TRUE,_xlfn._xlws.FILTER(plan[Event],plan[Date]=C5,""))</f>
-        <v/>
+        <v>Labor Day</v>
       </c>
       <c r="D6" s="16" t="str" cm="1">
         <f t="array" ref="D6">_xlfn.TEXTJOIN(CHAR(10),TRUE,_xlfn._xlws.FILTER(plan[Event],plan[Date]=D5,""))</f>
@@ -2828,12 +2961,12 @@
     <mergeCell ref="D14:H14"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:H11 B13:C13">
-    <cfRule type="expression" dxfId="13" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>AND(DAY(B11)&gt;=1,DAY(B11)&lt;=15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:G3">
-    <cfRule type="expression" dxfId="12" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>DAY(B3)&gt;8</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3227,12 +3360,12 @@
     <mergeCell ref="D14:H14"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:H11 B13:C13">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>AND(DAY(B11)&gt;=1,DAY(B11)&lt;=15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:G3">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>DAY(B3)&gt;8</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3391,7 +3524,7 @@
       <c r="A6" s="1"/>
       <c r="B6" s="16" t="str" cm="1">
         <f t="array" ref="B6">_xlfn.TEXTJOIN(CHAR(10),TRUE,_xlfn._xlws.FILTER(plan[Event],plan[Date]=B5,""))</f>
-        <v/>
+        <v>Daylight Savings Ends</v>
       </c>
       <c r="C6" s="16" t="str" cm="1">
         <f t="array" ref="C6">_xlfn.TEXTJOIN(CHAR(10),TRUE,_xlfn._xlws.FILTER(plan[Event],plan[Date]=C5,""))</f>
@@ -3626,12 +3759,12 @@
     <mergeCell ref="D14:H14"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:H11 B13:C13">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>AND(DAY(B11)&gt;=1,DAY(B11)&lt;=15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:G3">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>DAY(B3)&gt;8</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3918,7 +4051,7 @@
       </c>
       <c r="F10" s="16" t="str" cm="1">
         <f t="array" ref="F10">_xlfn.TEXTJOIN(CHAR(10),TRUE,_xlfn._xlws.FILTER(plan[Event],plan[Date]=F9,""))</f>
-        <v/>
+        <v>Thanksgiving</v>
       </c>
       <c r="G10" s="16" t="str" cm="1">
         <f t="array" ref="G10">_xlfn.TEXTJOIN(CHAR(10),TRUE,_xlfn._xlws.FILTER(plan[Event],plan[Date]=G9,""))</f>
@@ -4025,12 +4158,12 @@
     <mergeCell ref="D14:H14"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:H11 B13:C13">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>AND(DAY(B11)&gt;=1,DAY(B11)&lt;=15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:G3">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>DAY(B3)&gt;8</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4048,7 +4181,7 @@
   </sheetPr>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -4321,7 +4454,7 @@
       </c>
       <c r="C10" s="16" t="str" cm="1">
         <f t="array" ref="C10">_xlfn.TEXTJOIN(CHAR(10),TRUE,_xlfn._xlws.FILTER(plan[Event],plan[Date]=C9,""))</f>
-        <v/>
+        <v>Martin Luther King Jr. Day</v>
       </c>
       <c r="D10" s="16" t="str" cm="1">
         <f t="array" ref="D10">_xlfn.TEXTJOIN(CHAR(10),TRUE,_xlfn._xlws.FILTER(plan[Event],plan[Date]=D9,""))</f>
@@ -4440,12 +4573,12 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B11:H11 B13:C13">
-    <cfRule type="expression" dxfId="29" priority="24">
+    <cfRule type="expression" dxfId="23" priority="24">
       <formula>AND(DAY(B11)&gt;=1,DAY(B11)&lt;=15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:G3">
-    <cfRule type="expression" dxfId="28" priority="23">
+    <cfRule type="expression" dxfId="22" priority="23">
       <formula>DAY(B3)&gt;8</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4878,12 +5011,12 @@
     <mergeCell ref="D14:H14"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:H11 B13:C13">
-    <cfRule type="expression" dxfId="27" priority="2">
+    <cfRule type="expression" dxfId="21" priority="2">
       <formula>AND(DAY(B11)&gt;=1,DAY(B11)&lt;=15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:G3">
-    <cfRule type="expression" dxfId="26" priority="1">
+    <cfRule type="expression" dxfId="20" priority="1">
       <formula>DAY(B3)&gt;8</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5098,7 +5231,7 @@
       <c r="A8" s="1"/>
       <c r="B8" s="19" t="str" cm="1">
         <f t="array" ref="B8">_xlfn.TEXTJOIN(CHAR(10),TRUE,_xlfn._xlws.FILTER(plan[Event],plan[Date]=B7,""))</f>
-        <v/>
+        <v>Daylight Savings Starts</v>
       </c>
       <c r="C8" s="19" t="str" cm="1">
         <f t="array" ref="C8">_xlfn.TEXTJOIN(CHAR(10),TRUE,_xlfn._xlws.FILTER(plan[Event],plan[Date]=C7,""))</f>
@@ -5277,12 +5410,12 @@
     <mergeCell ref="D14:H14"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:H11 B13:C13">
-    <cfRule type="expression" dxfId="25" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>AND(DAY(B11)&gt;=1,DAY(B11)&lt;=15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:G3">
-    <cfRule type="expression" dxfId="24" priority="1">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>DAY(B3)&gt;8</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5676,12 +5809,12 @@
     <mergeCell ref="D14:H14"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:H11 B13:C13">
-    <cfRule type="expression" dxfId="23" priority="2">
+    <cfRule type="expression" dxfId="17" priority="2">
       <formula>AND(DAY(B11)&gt;=1,DAY(B11)&lt;=15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:G3">
-    <cfRule type="expression" dxfId="22" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>DAY(B3)&gt;8</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5840,7 +5973,7 @@
       <c r="A6" s="1"/>
       <c r="B6" s="16" t="str" cm="1">
         <f t="array" ref="B6">_xlfn.TEXTJOIN(CHAR(10),TRUE,_xlfn._xlws.FILTER(plan[Event],plan[Date]=B5,""))</f>
-        <v/>
+        <v>Mother's Day</v>
       </c>
       <c r="C6" s="16" t="str" cm="1">
         <f t="array" ref="C6">_xlfn.TEXTJOIN(CHAR(10),TRUE,_xlfn._xlws.FILTER(plan[Event],plan[Date]=C5,""))</f>
@@ -6013,7 +6146,8 @@
       </c>
       <c r="C12" s="19" t="str" cm="1">
         <f t="array" ref="C12">_xlfn.TEXTJOIN(CHAR(10),TRUE,_xlfn._xlws.FILTER(plan[Event],plan[Date]=C11,""))</f>
-        <v>Yuga Aoyama's 17th Birthday</v>
+        <v>Memorial Day
+Yuga Aoyama's 17th Birthday</v>
       </c>
       <c r="D12" s="19" t="str" cm="1">
         <f t="array" ref="D12">_xlfn.TEXTJOIN(CHAR(10),TRUE,_xlfn._xlws.FILTER(plan[Event],plan[Date]=D11,""))</f>
@@ -6076,12 +6210,12 @@
     <mergeCell ref="D14:H14"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:H11 B13:C13">
-    <cfRule type="expression" dxfId="21" priority="2">
+    <cfRule type="expression" dxfId="15" priority="2">
       <formula>AND(DAY(B11)&gt;=1,DAY(B11)&lt;=15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:G3">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>DAY(B3)&gt;8</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6188,7 +6322,8 @@
       </c>
       <c r="C4" s="19" t="str" cm="1">
         <f t="array" ref="C4">_xlfn.TEXTJOIN(CHAR(10),TRUE,_xlfn._xlws.FILTER(plan[Event],plan[Date]=C3,""))</f>
-        <v>Yuga Aoyama's 17th Birthday</v>
+        <v>Memorial Day
+Yuga Aoyama's 17th Birthday</v>
       </c>
       <c r="D4" s="19" t="str" cm="1">
         <f t="array" ref="D4">_xlfn.TEXTJOIN(CHAR(10),TRUE,_xlfn._xlws.FILTER(plan[Event],plan[Date]=D3,""))</f>
@@ -6353,6 +6488,7 @@
       <c r="B10" s="16" t="str" cm="1">
         <f t="array" ref="B10">_xlfn.TEXTJOIN(CHAR(10),TRUE,_xlfn._xlws.FILTER(plan[Event],plan[Date]=B9,""))</f>
         <v>Juneteenth
+Father's Day
 Rikido Sato's 17th Birthday</v>
       </c>
       <c r="C10" s="16" t="str" cm="1">
@@ -6476,12 +6612,12 @@
     <mergeCell ref="D14:H14"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:H11 B13:C13">
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>AND(DAY(B11)&gt;=1,DAY(B11)&lt;=15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:G3">
-    <cfRule type="expression" dxfId="18" priority="1">
+    <cfRule type="expression" dxfId="12" priority="1">
       <formula>DAY(B3)&gt;8</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6875,12 +7011,12 @@
     <mergeCell ref="D14:H14"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:H11 B13:C13">
-    <cfRule type="expression" dxfId="17" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>AND(DAY(B11)&gt;=1,DAY(B11)&lt;=15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:G3">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>DAY(B3)&gt;8</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7259,7 +7395,7 @@
       </c>
       <c r="C14" s="16" t="str" cm="1">
         <f t="array" ref="C14">_xlfn.TEXTJOIN(CHAR(10),TRUE,_xlfn._xlws.FILTER(plan[Event],plan[Date]=C13,""))</f>
-        <v/>
+        <v>Labor Day</v>
       </c>
       <c r="D14" s="36"/>
       <c r="E14" s="36"/>
@@ -7274,12 +7410,12 @@
     <mergeCell ref="D14:H14"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:H11 B13:C13">
-    <cfRule type="expression" dxfId="15" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>AND(DAY(B11)&gt;=1,DAY(B11)&lt;=15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:G3">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>DAY(B3)&gt;8</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>